<commit_message>
this includes the push of listners
</commit_message>
<xml_diff>
--- a/NINJACRMPROJECT/src/test/resources/E38_updated.xlsx
+++ b/NINJACRMPROJECT/src/test/resources/E38_updated.xlsx
@@ -632,7 +632,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Seshupriya</t>
+          <t>priya</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -715,7 +715,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Vendor_93777 - (Electronics)</t>
+          <t>Vendor_78713 - (Electronics)</t>
         </is>
       </c>
     </row>

</xml_diff>